<commit_message>
This is second push
</commit_message>
<xml_diff>
--- a/FileOutputData/Fileoutput.xlsx
+++ b/FileOutputData/Fileoutput.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
   <si>
     <t>Doctor Name</t>
   </si>
@@ -20,22 +20,34 @@
     <t>Doctor Description</t>
   </si>
   <si>
-    <t>Ms. Nutan Korgaonkar</t>
+    <t>Ms. Ashwini B N</t>
   </si>
   <si>
-    <t>A</t>
+    <t>Ms Ashwini B N is a Speech and Language Therapist with broad knowledge of Communication disorders. Resourceful and quick to identify and assess speech and language disorders. Applies appropriate and customized techniques to provide excellent therapeutic management to clients. [shrink]</t>
   </si>
   <si>
-    <t>Ms. Komal L Renuke</t>
+    <t>Ms. Rashmi Viswamurthy Krishna Rao</t>
   </si>
   <si>
-    <t>Ms. Komal L Renuke is a Audiologist and Speech Therapist in Powai, Mumbai and has an experience of 16 years in these fields. Ms. Komal L Renuke practices at Dr L H Hiranandani Hospital in Powai, Mumbai. She completed BASLP from Maharashtra Universtity of Health Sciences, Nashik in 2008. [shrink]</t>
+    <t>Ms Rashmi Viswamurthy Krishna Rao is a speech-language pathologist with over 15 years of experience in rehabilitation and healthcare in the clinical, NGO, and education sectors. Counselled over 2000 patients between the ages of 3 and 20 with</t>
   </si>
   <si>
-    <t>Mr. Piyush Gujarathi</t>
+    <t>Ms. Simantinee Chakraborty</t>
   </si>
   <si>
-    <t>Mr Piyush Gujarathi is an Audiologist and Speech Therapist in Matunga, Mumbai and has an experience of 6 years in the field of Speech, Hearing and Swallowing. Mr Piyush Gujarathi practices at SHADES Center of Excellance in Parel Mumbai, Shreeji Speech And Hearing Clinic in Matunga, Mumbai, Sushrusha Hospital in Dadar, Surya Hospital in Santacruz, Mumbai and Global Hospital, Parel.</t>
+    <t>Completed Master of Audiology and Speech Language Pathology from Ali Yavar Jung National Institute for the Hearing Handicapped, Eastern Regional Centre.</t>
+  </si>
+  <si>
+    <t>Ms. Madhura P Pradeep</t>
+  </si>
+  <si>
+    <t>Ms. Madhura P Pradeep is a Speech Therapist and Audiologist in Banashankari 2nd Stage, Bangalore and has an experience of 7 years in these fields. Ms. Madhura P Pradeep practices at Meenakshi ENT Speciality Hospital (MENTS) in Banashankari 2nd Stage, Bangalore. She completed BASLP from Bangalore University in 2017. [shrink]</t>
+  </si>
+  <si>
+    <t>Mr. Badrinath S N</t>
+  </si>
+  <si>
+    <t>Mr. Badrinath S N is a Audiologist and Speech Therapist in Banashankari 2nd Stage, Bangalore and has an experience of 24 years in these fields. Mr. Badrinath S N practices at Meenakshi ENT Speciality Hospital (MENTS) in Banashankari 2nd Stage, Bangalore and Vibrant Rehabilitation Centre in Banashankari 2nd Stage, Bangalore. He completed BSc. - Hearing, Language and Speech from Manipal Academy Of Higher Education, Manipal, India in 2000 and MSc. - Speech and Hearing from Mangalore University in 2003.</t>
   </si>
 </sst>
 </file>
@@ -80,7 +92,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:B4"/>
+  <dimension ref="A1:B6"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true"/>
   </sheetViews>
@@ -118,6 +130,22 @@
         <v>7</v>
       </c>
     </row>
+    <row r="5">
+      <c r="A5" t="s" s="0">
+        <v>8</v>
+      </c>
+      <c r="B5" t="s" s="0">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="s" s="0">
+        <v>10</v>
+      </c>
+      <c r="B6" t="s" s="0">
+        <v>11</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>

</xml_diff>